<commit_message>
Analysis of growth data
</commit_message>
<xml_diff>
--- a/TEST/SOBOL_BIG/7F_48_WELL_COMPLETE_FILLING_M9_LIPOQQQ/surrogate_modelling/compare.xlsx
+++ b/TEST/SOBOL_BIG/7F_48_WELL_COMPLETE_FILLING_M9_LIPOQQQ/surrogate_modelling/compare.xlsx
@@ -393,338 +393,338 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2">
-        <v>0.9804109092282964</v>
+        <v>0.8544378796644995</v>
       </c>
       <c r="B2">
-        <v>1.00155777791388</v>
+        <v>0.8568587807719603</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>0.95256418570582</v>
+        <v>0.6463411907890931</v>
       </c>
       <c r="B3">
-        <v>0.980961291165962</v>
+        <v>0.6508037365575856</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>0.9616055866854764</v>
+        <v>0.616621464201531</v>
       </c>
       <c r="B4">
-        <v>0.969320908971335</v>
+        <v>0.6196006649465076</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>0.981017789113474</v>
+        <v>0.8194018943245311</v>
       </c>
       <c r="B5">
-        <v>0.9856265844929345</v>
+        <v>0.8230693242384203</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>0.7583350155932368</v>
+        <v>0.0805354307539307</v>
       </c>
       <c r="B6">
-        <v>0.9185689033212515</v>
+        <v>0.08849797441731577</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>0.9392336650851844</v>
+        <v>0.96925716638757</v>
       </c>
       <c r="B7">
-        <v>0.9390723024211897</v>
+        <v>0.9640248577244662</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>1.01910435098856</v>
+        <v>1.298841514114648</v>
       </c>
       <c r="B8">
-        <v>1.009168628350987</v>
+        <v>1.285869942372226</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9">
-        <v>1.041967571027262</v>
+        <v>1.753943295583375</v>
       </c>
       <c r="B9">
-        <v>1.032803184102502</v>
+        <v>1.744144833335414</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10">
-        <v>0.9601041386044776</v>
+        <v>0.6003913602122007</v>
       </c>
       <c r="B10">
-        <v>0.9566077975039455</v>
+        <v>0.603435823035954</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11">
-        <v>0.971119986981879</v>
+        <v>1.310652557793934</v>
       </c>
       <c r="B11">
-        <v>0.9764252671780937</v>
+        <v>1.307704649210073</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12">
-        <v>1.04204572901701</v>
+        <v>1.750731214159401</v>
       </c>
       <c r="B12">
-        <v>1.006493948582908</v>
+        <v>1.738927247565891</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13">
-        <v>1.039407007226883</v>
+        <v>1.733198432686658</v>
       </c>
       <c r="B13">
-        <v>1.029585917618185</v>
+        <v>1.721132472644895</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14">
-        <v>1.030161660989599</v>
+        <v>1.514918593871193</v>
       </c>
       <c r="B14">
-        <v>1.025025625572892</v>
+        <v>1.506946016148416</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15">
-        <v>0.9879706187460132</v>
+        <v>0.9124105864632828</v>
       </c>
       <c r="B15">
-        <v>0.987499122566271</v>
+        <v>0.9117524573638238</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16">
-        <v>0.9943165386058972</v>
+        <v>0.9652833326741588</v>
       </c>
       <c r="B16">
-        <v>0.9807549675433679</v>
+        <v>0.9594030572056931</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17">
-        <v>0.9668275867458672</v>
+        <v>0.6519566776739463</v>
       </c>
       <c r="B17">
-        <v>0.9623774147511445</v>
+        <v>0.6558769406337663</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18">
-        <v>0.960456635965943</v>
+        <v>0.6436283712855808</v>
       </c>
       <c r="B18">
-        <v>0.9636910640943946</v>
+        <v>0.6450455588157792</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19">
-        <v>1.035724338408871</v>
+        <v>1.597932677876217</v>
       </c>
       <c r="B19">
-        <v>1.004852512483881</v>
+        <v>1.584705878787109</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20">
-        <v>0.9891208868766016</v>
+        <v>0.9069490511470674</v>
       </c>
       <c r="B20">
-        <v>0.9839765969015686</v>
+        <v>0.912686059895371</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21">
-        <v>0.969178284025965</v>
+        <v>0.7101530737634343</v>
       </c>
       <c r="B21">
-        <v>0.9610722277514244</v>
+        <v>0.7138587298365591</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22">
-        <v>0.8242616034182482</v>
+        <v>0.1413705257254187</v>
       </c>
       <c r="B22">
-        <v>0.9356357357365291</v>
+        <v>0.1501976737139035</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23">
-        <v>1.029086451937863</v>
+        <v>1.4913702792392</v>
       </c>
       <c r="B23">
-        <v>0.9962304881934094</v>
+        <v>1.474531607867737</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24">
-        <v>0.9701468643770992</v>
+        <v>0.681790817376478</v>
       </c>
       <c r="B24">
-        <v>0.9785806468726348</v>
+        <v>0.6852419275788471</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25">
-        <v>0.9822242041888384</v>
+        <v>0.8287310113894724</v>
       </c>
       <c r="B25">
-        <v>0.9842675101760621</v>
+        <v>0.8316630937330675</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26">
-        <v>1.018126873007233</v>
+        <v>1.287761039043411</v>
       </c>
       <c r="B26">
-        <v>0.9978441232759853</v>
+        <v>1.281951533063581</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27">
-        <v>0.8958090813408635</v>
+        <v>0.3093444057557265</v>
       </c>
       <c r="B27">
-        <v>0.9040613428697067</v>
+        <v>0.3130104681774866</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28">
-        <v>1.018925967312036</v>
+        <v>1.282200554881656</v>
       </c>
       <c r="B28">
-        <v>1.005774130066785</v>
+        <v>1.28780669613771</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29">
-        <v>0.9698474535587808</v>
+        <v>0.7520441022150447</v>
       </c>
       <c r="B29">
-        <v>0.9722316544785777</v>
+        <v>0.7531660135440238</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30">
-        <v>0.9735352356560676</v>
+        <v>1.163541580838492</v>
       </c>
       <c r="B30">
-        <v>0.9764058554731792</v>
+        <v>1.157771411623605</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31">
-        <v>0.9645541637159446</v>
+        <v>0.6358393769419587</v>
       </c>
       <c r="B31">
-        <v>0.9667199549766351</v>
+        <v>0.6392176430679251</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32">
-        <v>0.9694125363829468</v>
+        <v>0.6906127335161945</v>
       </c>
       <c r="B32">
-        <v>0.9688586259148931</v>
+        <v>0.6900792722450098</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33">
-        <v>0.9795226604017272</v>
+        <v>0.7695585959571494</v>
       </c>
       <c r="B33">
-        <v>0.9698600565232937</v>
+        <v>0.7643755423797318</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34">
-        <v>0.7621573952864661</v>
+        <v>0.0468689095057648</v>
       </c>
       <c r="B34">
-        <v>0.9841194146006024</v>
+        <v>0.06971745368735227</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35">
-        <v>1.000725671052213</v>
+        <v>1.0164714988704</v>
       </c>
       <c r="B35">
-        <v>0.9960743157614982</v>
+        <v>1.011373846772858</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36">
-        <v>0.9029714018089948</v>
+        <v>0.3763628084380087</v>
       </c>
       <c r="B36">
-        <v>0.9805849319477857</v>
+        <v>0.3839347535113792</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37">
-        <v>1.019414073506677</v>
+        <v>1.30186507690716</v>
       </c>
       <c r="B37">
-        <v>1.014909385373074</v>
+        <v>1.296988677021973</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38">
-        <v>0.9041361505142106</v>
+        <v>0.398555750789446</v>
       </c>
       <c r="B38">
-        <v>0.9277039201999935</v>
+        <v>0.405733442907917</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39">
-        <v>0.9705239312525292</v>
+        <v>0.7199799374896158</v>
       </c>
       <c r="B39">
-        <v>0.991242514960775</v>
+        <v>0.7258200266249029</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40">
-        <v>0.988732400308986</v>
+        <v>0.9171691541809092</v>
       </c>
       <c r="B40">
-        <v>0.9884431531185602</v>
+        <v>0.9143059459606744</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41">
-        <v>0.9544364454470065</v>
+        <v>0.5582211534847016</v>
       </c>
       <c r="B41">
-        <v>0.9583011294857773</v>
+        <v>0.5564744892975657</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42">
-        <v>0.979280390497318</v>
+        <v>0.7880253087745966</v>
       </c>
       <c r="B42">
-        <v>0.9770489503815196</v>
+        <v>0.7937830085106274</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
-        <v>0.9868873859433897</v>
+        <v>0.8577585081917437</v>
       </c>
       <c r="B43">
-        <v>0.9777681006460717</v>
+        <v>0.8567376221429097</v>
       </c>
     </row>
   </sheetData>

</xml_diff>